<commit_message>
feat: Enhance smart column mapping tool with detailed comparison and AI guidance
</commit_message>
<xml_diff>
--- a/tests/test_data/target_local.xlsx
+++ b/tests/test_data/target_local.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Open Source</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Under Review</t>
+          <t>Needs Review</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,51 +492,34 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/src/api/http-client.json</t>
+          <t>/src/api/new-endpoint.json</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pending Review</t>
+          <t>New</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Axios HTTP Client</t>
+          <t>API Endpoint</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/src/utils/date-formatter.js</t>
+          <t>/src/utils/validator.js</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Open Source</t>
+          <t>Approved</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Moment.js</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>/src/components/charts/bar-chart.css</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Approved</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Chart.js</t>
+          <t>Input Validator</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Add custom chat mode for Excel file operations and update Excel processing tools
</commit_message>
<xml_diff>
--- a/tests/test_data/target_local.xlsx
+++ b/tests/test_data/target_local.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Approved</t>
+          <t>Open Source</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -463,7 +463,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Needs Review</t>
+          <t>Under Review</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,34 +492,51 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>/src/api/new-endpoint.json</t>
+          <t>/src/api/http-client.json</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>New</t>
+          <t>Pending Review</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>API Endpoint</t>
+          <t>Axios HTTP Client</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>/src/utils/validator.js</t>
+          <t>/src/utils/date-formatter.js</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Open Source</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Moment.js</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/src/components/charts/bar-chart.css</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Approved</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Input Validator</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Chart.js</t>
         </is>
       </c>
     </row>

</xml_diff>